<commit_message>
MIP funcionando, tocando CVX en 4node
</commit_message>
<xml_diff>
--- a/4node_spain/output_a.xlsx
+++ b/4node_spain/output_a.xlsx
@@ -478,7 +478,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>4.478308985051494</v>
+        <v>2.257119139371683</v>
       </c>
     </row>
     <row r="4">
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>1.696207746594563</v>
+        <v>0.8998700214674639</v>
       </c>
     </row>
     <row r="5">
@@ -510,10 +510,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>4.478308985051494</v>
+        <v>2.257119139371683</v>
       </c>
       <c r="D5" t="n">
-        <v>1.696207746594563</v>
+        <v>0.8998700214674639</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
add cvx model for 4 node
</commit_message>
<xml_diff>
--- a/4node_spain/output_a.xlsx
+++ b/4node_spain/output_a.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,31 @@
           <t>i4</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>i5</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>i6</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>i7</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>i8</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>i9</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -453,12 +478,27 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.00178640640744647</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.001783378767856305</v>
       </c>
       <c r="E2" t="n">
+        <v>0.001183898155703645</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -469,16 +509,31 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>0.00178640640744647</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.001436737742693641</v>
       </c>
       <c r="E3" t="n">
-        <v>2.257119139371683</v>
+        <v>5.786744453957676</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -488,16 +543,31 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>0.001783378767856305</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>0.001436737742693641</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8998700214674639</v>
+        <v>2.257054535163327</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -507,15 +577,200 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.001183898155703645</v>
       </c>
       <c r="C5" t="n">
-        <v>2.257119139371683</v>
+        <v>5.786744453957676</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8998700214674639</v>
+        <v>2.257054535163327</v>
       </c>
       <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>i5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>i6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>i7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>i8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>i9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
elimino beta de mip
</commit_message>
<xml_diff>
--- a/4node_spain/output_a.xlsx
+++ b/4node_spain/output_a.xlsx
@@ -478,13 +478,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00178640640744647</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001783378767856305</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.001183898155703645</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -509,16 +509,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.00178640640744647</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001436737742693641</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>5.786744453957676</v>
+        <v>2.257119139371683</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.001783378767856305</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001436737742693641</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>2.257054535163327</v>
+        <v>0.8998700276285728</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -577,13 +577,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.001183898155703645</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>5.786744453957676</v>
+        <v>2.257119139371683</v>
       </c>
       <c r="D5" t="n">
-        <v>2.257054535163327</v>
+        <v>0.8998700276285728</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
blo working on 4 node
</commit_message>
<xml_diff>
--- a/4node_spain/output_a.xlsx
+++ b/4node_spain/output_a.xlsx
@@ -478,13 +478,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1.711173756007756e-07</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>5.049777682986309e-09</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>3.847902911326734e-09</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -509,16 +509,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1.711173756007756e-07</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>7.043876027046637e-09</v>
       </c>
       <c r="E3" t="n">
-        <v>2.257119139371683</v>
+        <v>2.218573043980729</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>5.049777682986309e-09</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>7.043876027046637e-09</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8998700276285728</v>
+        <v>0.8517350933034392</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -577,13 +577,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>3.847902911326734e-09</v>
       </c>
       <c r="C5" t="n">
-        <v>2.257119139371683</v>
+        <v>2.218573043980729</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8998700276285728</v>
+        <v>0.8517350933034392</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
working on 6 node
</commit_message>
<xml_diff>
--- a/4node_spain/output_a.xlsx
+++ b/4node_spain/output_a.xlsx
@@ -478,13 +478,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>1.711173756007756e-07</v>
+        <v>1.724404365356792e-05</v>
       </c>
       <c r="D2" t="n">
-        <v>5.049777682986309e-09</v>
+        <v>9.871345059498339e-07</v>
       </c>
       <c r="E2" t="n">
-        <v>3.847902911326734e-09</v>
+        <v>7.033013450984647e-07</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -509,16 +509,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.711173756007756e-07</v>
+        <v>1.724404365356792e-05</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>7.043876027046637e-09</v>
+        <v>1.974535298499556e-06</v>
       </c>
       <c r="E3" t="n">
-        <v>2.218573043980729</v>
+        <v>2.213103850403893</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -543,16 +543,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.049777682986309e-09</v>
+        <v>9.871345059498339e-07</v>
       </c>
       <c r="C4" t="n">
-        <v>7.043876027046637e-09</v>
+        <v>1.974535298499556e-06</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8517350933034392</v>
+        <v>0.8572568171758366</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -577,13 +577,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.847902911326734e-09</v>
+        <v>7.033013450984647e-07</v>
       </c>
       <c r="C5" t="n">
-        <v>2.218573043980729</v>
+        <v>2.213103850403893</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8517350933034392</v>
+        <v>0.8572568171758366</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>

</xml_diff>